<commit_message>
Tile neighbours set, but not the prefabs
</commit_message>
<xml_diff>
--- a/Unity Files/Tiles Ref.xlsx
+++ b/Unity Files/Tiles Ref.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="10">
   <si>
     <t>Plains</t>
   </si>
@@ -97,11 +97,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,7 +419,7 @@
   <dimension ref="A1:AD30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="AD29" sqref="AD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,52 +439,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1" t="s">
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1" t="s">
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1" t="s">
+      <c r="R1" s="3"/>
+      <c r="S1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1" t="s">
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1" t="s">
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1" t="s">
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AD1" s="1"/>
+      <c r="AD1" s="3"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C2">
@@ -585,9 +585,6 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
       <c r="Q3" t="s">
         <v>9</v>
       </c>
@@ -614,16 +611,13 @@
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
         <v>9</v>
       </c>
       <c r="Q4" t="s">
@@ -637,8 +631,11 @@
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
@@ -655,13 +652,13 @@
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="Q6" t="s">
@@ -678,10 +675,10 @@
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
       <c r="G7" t="s">
         <v>9</v>
       </c>
@@ -708,11 +705,11 @@
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
       <c r="H8" t="s">
         <v>9</v>
       </c>
@@ -739,12 +736,12 @@
       <c r="B9">
         <v>3</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
       <c r="I9" t="s">
         <v>9</v>
       </c>
@@ -752,6 +749,18 @@
         <v>9</v>
       </c>
       <c r="K9" t="s">
+        <v>9</v>
+      </c>
+      <c r="S9" t="s">
+        <v>9</v>
+      </c>
+      <c r="T9" t="s">
+        <v>9</v>
+      </c>
+      <c r="U9" t="s">
+        <v>9</v>
+      </c>
+      <c r="V9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -759,13 +768,13 @@
       <c r="B10">
         <v>4</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
       <c r="J10" t="s">
         <v>9</v>
       </c>
@@ -792,14 +801,14 @@
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
       <c r="K11" t="s">
         <v>9</v>
       </c>
@@ -823,15 +832,15 @@
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
       <c r="L12" t="s">
         <v>9</v>
       </c>
@@ -843,16 +852,16 @@
       <c r="B13">
         <v>3</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
       <c r="M13" t="s">
         <v>9</v>
       </c>
@@ -864,17 +873,17 @@
       <c r="B14">
         <v>4</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
       <c r="N14" t="s">
         <v>9</v>
       </c>
@@ -886,18 +895,18 @@
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
       <c r="AB15" t="s">
         <v>9</v>
       </c>
@@ -906,19 +915,19 @@
       <c r="B16">
         <v>2</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
       <c r="AB16" t="s">
         <v>9</v>
       </c>
@@ -930,20 +939,20 @@
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
       <c r="S17" t="s">
         <v>9</v>
       </c>
@@ -961,21 +970,21 @@
       <c r="B18">
         <v>2</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
       <c r="S18" t="s">
         <v>9</v>
       </c>
@@ -996,34 +1005,28 @@
       <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
+      <c r="C19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
       <c r="S19" t="s">
         <v>9</v>
       </c>
       <c r="T19" t="s">
-        <v>9</v>
-      </c>
-      <c r="U19" t="s">
-        <v>9</v>
-      </c>
-      <c r="V19" t="s">
         <v>9</v>
       </c>
       <c r="W19" t="s">
@@ -1046,30 +1049,27 @@
       <c r="B20">
         <v>2</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
       <c r="T20" t="s">
         <v>9</v>
       </c>
       <c r="U20" t="s">
-        <v>9</v>
-      </c>
-      <c r="V20" t="s">
         <v>9</v>
       </c>
       <c r="W20" t="s">
@@ -1083,24 +1083,24 @@
       <c r="B21">
         <v>3</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
       <c r="U21" t="s">
         <v>9</v>
       </c>
@@ -1118,32 +1118,26 @@
       <c r="B22">
         <v>4</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
       <c r="V22" t="s">
-        <v>9</v>
-      </c>
-      <c r="W22" t="s">
-        <v>9</v>
-      </c>
-      <c r="X22" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1154,52 +1148,52 @@
       <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
-      <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>2</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
-      <c r="T24" s="2"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1208,28 +1202,31 @@
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
-      <c r="W25" s="2"/>
-      <c r="X25" s="2"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" t="s">
+        <v>9</v>
+      </c>
       <c r="Z25" t="s">
         <v>9</v>
       </c>
@@ -1244,29 +1241,29 @@
       <c r="B26">
         <v>2</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
-      <c r="T26" s="2"/>
-      <c r="U26" s="2"/>
-      <c r="V26" s="2"/>
-      <c r="W26" s="2"/>
-      <c r="X26" s="2"/>
-      <c r="Y26" s="2"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
       <c r="Z26" t="s">
         <v>9</v>
       </c>
@@ -1284,30 +1281,30 @@
       <c r="B27">
         <v>3</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
-      <c r="T27" s="2"/>
-      <c r="U27" s="2"/>
-      <c r="V27" s="2"/>
-      <c r="W27" s="2"/>
-      <c r="X27" s="2"/>
-      <c r="Y27" s="2"/>
-      <c r="Z27" s="2"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
       <c r="AA27" t="s">
         <v>9</v>
       </c>
@@ -1319,31 +1316,31 @@
       <c r="B28">
         <v>4</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-      <c r="R28" s="2"/>
-      <c r="S28" s="2"/>
-      <c r="T28" s="2"/>
-      <c r="U28" s="2"/>
-      <c r="V28" s="2"/>
-      <c r="W28" s="2"/>
-      <c r="X28" s="2"/>
-      <c r="Y28" s="2"/>
-      <c r="Z28" s="2"/>
-      <c r="AA28" s="2"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
       <c r="AB28" t="s">
         <v>9</v>
       </c>
@@ -1355,32 +1352,32 @@
       <c r="B29">
         <v>1</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
-      <c r="T29" s="2"/>
-      <c r="U29" s="2"/>
-      <c r="V29" s="2"/>
-      <c r="W29" s="2"/>
-      <c r="X29" s="2"/>
-      <c r="Y29" s="2"/>
-      <c r="Z29" s="2"/>
-      <c r="AA29" s="2"/>
-      <c r="AB29" s="2"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
       <c r="AD29" t="s">
         <v>9</v>
       </c>
@@ -1389,33 +1386,33 @@
       <c r="B30">
         <v>2</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
-      <c r="R30" s="2"/>
-      <c r="S30" s="2"/>
-      <c r="T30" s="2"/>
-      <c r="U30" s="2"/>
-      <c r="V30" s="2"/>
-      <c r="W30" s="2"/>
-      <c r="X30" s="2"/>
-      <c r="Y30" s="2"/>
-      <c r="Z30" s="2"/>
-      <c r="AA30" s="2"/>
-      <c r="AB30" s="2"/>
-      <c r="AC30" s="2"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>